<commit_message>
Excel Update and Scene Update
Updated FTOC and added boundaries.
</commit_message>
<xml_diff>
--- a/Magnum Prandium.xlsx
+++ b/Magnum Prandium.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Genzo\Documents\Git\magnum-prandium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A6542A-80D9-4693-8697-330C5CCF7E49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B73575-56DA-4E12-9C3E-9B7C53DD8E01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18495" windowHeight="8235" xr2:uid="{F3EF63F0-F62E-4576-B136-89CA54175D03}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="45">
   <si>
     <t>Movement</t>
   </si>
@@ -156,13 +156,22 @@
   </si>
   <si>
     <t>Dash</t>
+  </si>
+  <si>
+    <t>Gameover Condition</t>
+  </si>
+  <si>
+    <t>Win Condition</t>
+  </si>
+  <si>
+    <t>Enemy Asset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +186,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,8 +212,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -291,12 +312,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,12 +392,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -696,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BDD899-7C62-4415-B780-8703A6AA318C}">
-  <dimension ref="A14:G44"/>
+  <dimension ref="A14:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,16 +803,16 @@
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="14" t="s">
+      <c r="F15" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -760,8 +834,8 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="7" t="s">
-        <v>20</v>
+      <c r="D17" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>6</v>
@@ -770,96 +844,96 @@
         <v>10</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="7" t="s">
+      <c r="F20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="6" t="s">
-        <v>14</v>
+      <c r="D22" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="D23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>10</v>
+      <c r="F23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>7</v>
@@ -868,138 +942,138 @@
         <v>11</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="D25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="5" t="s">
+      <c r="F25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="13" t="s">
+      <c r="D26" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>12</v>
+      <c r="F26" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="7" t="s">
-        <v>22</v>
+      <c r="D27" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="6" t="s">
+      <c r="E32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D33" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="5" t="s">
+      <c r="E33" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>9</v>
@@ -1013,7 +1087,7 @@
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>9</v>
@@ -1027,27 +1101,27 @@
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="6" t="s">
-        <v>38</v>
+      <c r="D37" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>10</v>
@@ -1055,27 +1129,27 @@
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D39" s="6" t="s">
-        <v>19</v>
+      <c r="D39" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>10</v>
@@ -1083,79 +1157,121 @@
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D44" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D41" s="7" t="s">
+      <c r="E44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D45" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D42" s="7" t="s">
+      <c r="E45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D43" s="7" t="s">
+      <c r="E46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D44" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="9" t="s">
+      <c r="E47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="9" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="D15:G44">
-    <sortCondition ref="E15:E44" customList="C,I,U"/>
-    <sortCondition ref="F15:F44" customList="H,M,L"/>
-    <sortCondition ref="G15:G44" customList="H,M,L"/>
+  <sortState ref="D15:G47">
+    <sortCondition ref="E15:E47" customList="C,I,U"/>
+    <sortCondition ref="F15:F47" customList="H,M,L"/>
+    <sortCondition ref="G15:G47" customList="H,M,L"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>